<commit_message>
Added filetype check to upload roles just in case
</commit_message>
<xml_diff>
--- a/WebBasedEvaluations/Program documents/Upload_Roles.xlsx
+++ b/WebBasedEvaluations/Program documents/Upload_Roles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Program documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62EEEC9-4EB4-4ED0-A864-8818F5FD8C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDDC477-A760-43E6-A94A-B414E80517F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>ROLENAME</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>ADMIN</t>
+  </si>
+  <si>
+    <t>FileType:</t>
+  </si>
+  <si>
+    <t>Role Template</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,9 +445,11 @@
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +483,14 @@
       <c r="K1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -511,7 +525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -531,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -551,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -586,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -606,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -626,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -646,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -666,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -686,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -706,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -741,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -761,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -781,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -816,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>

</xml_diff>